<commit_message>
Added support for return import flow and refactored related components.
</commit_message>
<xml_diff>
--- a/src/assets/import-templates/template_phieu_nhap_tra.xlsx
+++ b/src/assets/import-templates/template_phieu_nhap_tra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doanvinhphu/Documents/Study/FPTU/Ky-9/capstone-project/warehouse_frontend/src/assets/import-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD93405D-0FF5-FC49-BC29-8B5AEA7A8728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C9BAB6-56FE-FE41-9A7F-BBD447C55647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="19380" windowHeight="20980" xr2:uid="{9FA52C3A-7928-408F-877C-18AC7D4D703A}"/>
   </bookViews>
@@ -55,10 +55,10 @@
     <t>NHẬP TRẢ</t>
   </si>
   <si>
-    <t>Mã sản phẩm cụ thể</t>
+    <t>Giá trị cần nhập</t>
   </si>
   <si>
-    <t>Giá trị cần nhập</t>
+    <t>Mã sản phẩm tồn kho</t>
   </si>
 </sst>
 </file>
@@ -676,7 +676,7 @@
   <dimension ref="A1:C200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -738,10 +738,10 @@
         <v>0</v>
       </c>
       <c r="B9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>6</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1949,14 +1949,14 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A10:C200">
+  <conditionalFormatting sqref="A9:C200">
     <cfRule type="expression" dxfId="1" priority="1">
-      <formula>A10&lt;&gt;""</formula>
+      <formula>A9&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:C10 B11:C198 A11:A200">
+  <conditionalFormatting sqref="B11:C198 A11:A200">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>A9&lt;&gt;""</formula>
+      <formula>A11&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>